<commit_message>
added tax wedge explanation
</commit_message>
<xml_diff>
--- a/tax_wedge.xlsx
+++ b/tax_wedge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alain\Desktop\assignments\data_analyses\dataMadness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alain\Desktop\assignments\data_analyses\dataMadness\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5720ABE5-4DB4-49E2-BAA1-819D5D23D57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D972DF-887B-4E43-A53A-5C113E672CE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="1590" windowWidth="21352" windowHeight="14010" xr2:uid="{1060DA4E-5CE6-4862-AFF7-AFC993E8459F}"/>
   </bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644EF14D-F92E-4AAB-812E-ABAFF682CDF1}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
fixed country names and ;oaded tax rates
</commit_message>
<xml_diff>
--- a/tax_wedge.xlsx
+++ b/tax_wedge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alain\Desktop\assignments\data_analyses\dataMadness\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D972DF-887B-4E43-A53A-5C113E672CE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC90C43-3261-4923-916C-3C33CB5E2978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1590" windowWidth="21352" windowHeight="14010" xr2:uid="{1060DA4E-5CE6-4862-AFF7-AFC993E8459F}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="21352" windowHeight="14010" xr2:uid="{1060DA4E-5CE6-4862-AFF7-AFC993E8459F}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -168,6 +168,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -207,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -215,6 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -532,7 +536,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -553,7 +557,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>34.4</v>
       </c>
     </row>
@@ -561,7 +565,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>51</v>
       </c>
     </row>
@@ -569,7 +573,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>58.7</v>
       </c>
     </row>
@@ -577,7 +581,7 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>31.8</v>
       </c>
     </row>
@@ -585,7 +589,7 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -593,7 +597,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>45.7</v>
       </c>
     </row>
@@ -601,7 +605,7 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>41.2</v>
       </c>
     </row>
@@ -609,7 +613,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>41.2</v>
       </c>
     </row>
@@ -617,7 +621,7 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>48.8</v>
       </c>
     </row>
@@ -625,7 +629,7 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>54.1</v>
       </c>
     </row>
@@ -633,7 +637,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>51</v>
       </c>
     </row>
@@ -641,7 +645,7 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>46.7</v>
       </c>
     </row>
@@ -649,7 +653,7 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>44.6</v>
       </c>
     </row>
@@ -657,7 +661,7 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>37.4</v>
       </c>
     </row>
@@ -665,7 +669,7 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>41.8</v>
       </c>
     </row>
@@ -673,7 +677,7 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>32.6</v>
       </c>
     </row>
@@ -681,7 +685,7 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>54</v>
       </c>
     </row>
@@ -689,7 +693,7 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>35.1</v>
       </c>
     </row>
@@ -697,7 +701,7 @@
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>25.6</v>
       </c>
     </row>
@@ -705,7 +709,7 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>45.6</v>
       </c>
     </row>
@@ -713,7 +717,7 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>23.2</v>
       </c>
     </row>
@@ -721,7 +725,7 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>42.2</v>
       </c>
     </row>
@@ -729,7 +733,7 @@
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>24.3</v>
       </c>
     </row>
@@ -737,7 +741,7 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>41.6</v>
       </c>
     </row>
@@ -745,7 +749,7 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>36.1</v>
       </c>
     </row>
@@ -753,7 +757,7 @@
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>46.6</v>
       </c>
     </row>
@@ -761,7 +765,7 @@
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>43.6</v>
       </c>
     </row>
@@ -769,7 +773,7 @@
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>47</v>
       </c>
     </row>
@@ -777,7 +781,7 @@
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>43.9</v>
       </c>
     </row>
@@ -785,7 +789,7 @@
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>50.7</v>
       </c>
     </row>
@@ -793,7 +797,7 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>26.9</v>
       </c>
     </row>
@@ -801,7 +805,7 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>42.9</v>
       </c>
     </row>
@@ -809,7 +813,7 @@
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>37.200000000000003</v>
       </c>
     </row>
@@ -817,7 +821,7 @@
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>34.1</v>
       </c>
     </row>
@@ -825,7 +829,7 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>38.200000000000003</v>
       </c>
     </row>
@@ -833,7 +837,7 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>34.6</v>
       </c>
     </row>
@@ -841,7 +845,7 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>30.2</v>
       </c>
     </row>
@@ -849,7 +853,7 @@
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>38.299999999999997</v>
       </c>
     </row>
@@ -857,7 +861,7 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>26.1</v>
       </c>
     </row>
@@ -865,7 +869,7 @@
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -873,7 +877,7 @@
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>27.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dropped countries with unknown tax wedge
</commit_message>
<xml_diff>
--- a/tax_wedge.xlsx
+++ b/tax_wedge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alain\Desktop\assignments\data_analyses\dataMadness\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC90C43-3261-4923-916C-3C33CB5E2978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3443D7-8F5F-415E-8A4D-20392315379A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="21352" windowHeight="14010" xr2:uid="{1060DA4E-5CE6-4862-AFF7-AFC993E8459F}"/>
+    <workbookView xWindow="2940" yWindow="1590" windowWidth="21352" windowHeight="14010" xr2:uid="{1060DA4E-5CE6-4862-AFF7-AFC993E8459F}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>tax wedge 167% AW</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>South Africa</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>taxWedge</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B42"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -547,15 +547,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>34.4</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>51</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>58.7</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>31.8</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>8.3000000000000007</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>45.7</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>41.2</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>41.2</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>48.8</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>54.1</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>51</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3">
         <v>46.7</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
         <v>44.6</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3">
         <v>37.4</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
         <v>41.8</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>32.6</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>54</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3">
         <v>35.1</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3">
         <v>25.6</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="3">
         <v>45.6</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="3">
         <v>23.2</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3">
         <v>42.2</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3">
         <v>24.3</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3">
         <v>41.6</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3">
         <v>36.1</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3">
         <v>46.6</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3">
         <v>43.6</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="3">
         <v>47</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="3">
         <v>43.9</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" s="3">
         <v>50.7</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="3">
         <v>26.9</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="3">
         <v>42.9</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="3">
         <v>37.200000000000003</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3">
         <v>34.1</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="3">
         <v>38.200000000000003</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3">
         <v>34.6</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3">
         <v>30.2</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3">
         <v>38.299999999999997</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3">
         <v>26.1</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3">
         <v>8.1999999999999993</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3">
         <v>27.5</v>

</xml_diff>